<commit_message>
Improved side by side
</commit_message>
<xml_diff>
--- a/adhd_adults_diagnosis_SoF.xlsx
+++ b/adhd_adults_diagnosis_SoF.xlsx
@@ -535,12 +535,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>41 studies (Aita, 2018{#16}; Bakare, 2020{#45}; Bastiaens, 2017{#55}; Chiasson, 2012{#141}; Dakwar, 2012{#172}; Dunlop, 2018{#212}; Grogan, 2018{#323}; Harrison, 2019{#351}; Houston, 2011{#390}; Kessler, 2005{#442}; Kwan, 2024{#490}; Lancaster, 2018{#495}; Lewandowski, 2008{#525}; Liu, 2023{#536}; Luty, 2009{#555}; Marchant, 2015{#571}; McCann, 2004{#603}; Mehringer, 2002{#611}; Palmer, 2023{#685}; Pettersson, 2018{#711}; Reimherr, 2021{#757}; Reyes, 2019{#762}; Singh, 2015{#857}; Solanto, 2004{#870}; Ustun, 2017{#940}; van de Glind, 2013{#942}; Van Voorhees, 2011{#949}; Vizgaitis, 2023{#960}; Young, 2023{#1016}; Young, 2016{#1017}; Kumar, 2011{#4185}; Roy-Byrne, 1997{#4485}; Erhardt, 1999{#5176}; Kingston, 2013{#5349}; De Quiros, 2001{#10619}; Dvorsky, 2016{#10626}; Faraone, 2010{#10633}; Skirrow, 2013{#10752}; Knight, 2025{#11044}; Herman, 2025{#14009}; Kitsune, 2016{#14746})</t>
+          <t>40 studies (Aita, 2018{#16}; Bakare, 2020{#45}; Bastiaens, 2017{#55}; Chiasson, 2012{#141}; Dakwar, 2012{#172}; Dunlop, 2018{#212}; Grogan, 2018{#323}; Houston, 2011{#390}; Kessler, 2005{#442}; Kwan, 2024{#490}; Lancaster, 2018{#495}; Lewandowski, 2008{#525}; Liu, 2023{#536}; Luty, 2009{#555}; Marchant, 2015{#571}; McCann, 2004{#603}; Mehringer, 2002{#611}; Palmer, 2023{#685}; Pettersson, 2018{#711}; Reimherr, 2021{#757}; Reyes, 2019{#762}; Singh, 2015{#857}; Solanto, 2004{#870}; Ustun, 2017{#940}; van de Glind, 2013{#942}; Van Voorhees, 2011{#949}; Vizgaitis, 2023{#960}; Young, 2023{#1016}; Young, 2016{#1017}; Kumar, 2011{#4185}; Roy-Byrne, 1997{#4485}; Erhardt, 1999{#5176}; Kingston, 2013{#5349}; De Quiros, 2001{#10619}; Dvorsky, 2016{#10626}; Faraone, 2010{#10633}; Skirrow, 2013{#10752}; Knight, 2025{#11044}; Herman, 2025{#14009}; Kitsune, 2016{#14746})</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>100(#141, 490) to 14(#351)</t>
+          <t>100(#141, 490) to 28(#11044)</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>39 studies (Bakare, 2020{#45}; Bastiaens, 2017{#55}; Dakwar, 2012{#172}; Dunlop, 2018{#212}; Grogan, 2018{#323}; Harrison, 2019{#351}; Houston, 2011{#390}; Kessler, 2005{#442}; Kwan, 2024{#490}; Lancaster, 2018{#495}; Lewandowski, 2008{#525}; Liu, 2023{#536}; Luty, 2009{#555}; Marchant, 2015{#571}; McCann, 2004{#603}; Mehringer, 2002{#611}; Palmer, 2023{#685}; Pettersson, 2018{#711}; Reimherr, 2021{#757}; Reyes, 2019{#762}; Singh, 2015{#857}; Solanto, 2004{#870}; Ustun, 2017{#940}; van de Glind, 2013{#942}; Van Voorhees, 2011{#949}; Vizgaitis, 2023{#960}; Young, 2023{#1016}; Young, 2016{#1017}; Kumar, 2011{#4185}; Roy-Byrne, 1997{#4485}; Erhardt, 1999{#5176}; Kingston, 2013{#5349}; De Quiros, 2001{#10619}; Dvorsky, 2016{#10626}; Faraone, 2010{#10633}; Skirrow, 2013{#10752}; Knight, 2025{#11044}; Herman, 2025{#14009}; Kitsune, 2016{#14746})</t>
+          <t>38 studies (Bakare, 2020{#45}; Bastiaens, 2017{#55}; Dakwar, 2012{#172}; Dunlop, 2018{#212}; Grogan, 2018{#323}; Houston, 2011{#390}; Kessler, 2005{#442}; Kwan, 2024{#490}; Lancaster, 2018{#495}; Lewandowski, 2008{#525}; Liu, 2023{#536}; Luty, 2009{#555}; Marchant, 2015{#571}; McCann, 2004{#603}; Mehringer, 2002{#611}; Palmer, 2023{#685}; Pettersson, 2018{#711}; Reimherr, 2021{#757}; Reyes, 2019{#762}; Singh, 2015{#857}; Solanto, 2004{#870}; Ustun, 2017{#940}; van de Glind, 2013{#942}; Van Voorhees, 2011{#949}; Vizgaitis, 2023{#960}; Young, 2023{#1016}; Young, 2016{#1017}; Kumar, 2011{#4185}; Roy-Byrne, 1997{#4485}; Erhardt, 1999{#5176}; Kingston, 2013{#5349}; De Quiros, 2001{#10619}; Dvorsky, 2016{#10626}; Faraone, 2010{#10633}; Skirrow, 2013{#10752}; Knight, 2025{#11044}; Herman, 2025{#14009}; Kitsune, 2016{#14746})</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1759,12 +1759,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>23 studies (Abramson, 2023{#5}; Aita, 2018{#16}; Becke, 2023{#58}; Berger, 2021{#68}; Courrege, 2019{#164}; Harrison, 2019{#351}; Musso, 2016{#646}; Potts, 2022{#733}; Quinn, 2003{#745}; Ramachandran, 2019{#750}; Robinson, 2023{#777}; Smith, 2017{#863}; Sollman, 2010{#872}; Spenceley, 2022{#883}; Young, 2011{#1015}; Harrison, 2020{#4042}; Morey, 2019{#4321}; Williamson, 2014{#4702}; Fuermaier, 2016{#5208}; Suhr, 2011{#10849}; Fuermaier, 2024{#11004}; Robinson, 2025{#11099}; Robinson, 2023{#14273})</t>
+          <t>22 studies (Abramson, 2023{#5}; Aita, 2018{#16}; Becke, 2023{#58}; Berger, 2021{#68}; Courrege, 2019{#164}; Musso, 2016{#646}; Potts, 2022{#733}; Quinn, 2003{#745}; Ramachandran, 2019{#750}; Robinson, 2023{#777}; Smith, 2017{#863}; Sollman, 2010{#872}; Spenceley, 2022{#883}; Young, 2011{#1015}; Harrison, 2020{#4042}; Morey, 2019{#4321}; Williamson, 2014{#4702}; Fuermaier, 2016{#5208}; Suhr, 2011{#10849}; Fuermaier, 2024{#11004}; Robinson, 2025{#11099}; Robinson, 2023{#14273})</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>94(#745) to 24(#351, 10849)</t>
+          <t>94(#745) to 24(#10849)</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>21 studies (Abramson, 2023{#5}; Becke, 2023{#58}; Berger, 2021{#68}; Courrege, 2019{#164}; Harrison, 2019{#351}; Musso, 2016{#646}; Potts, 2022{#733}; Quinn, 2003{#745}; Ramachandran, 2019{#750}; Robinson, 2023{#777}; Smith, 2017{#863}; Sollman, 2010{#872}; Spenceley, 2022{#883}; Young, 2011{#1015}; Harrison, 2020{#4042}; Morey, 2019{#4321}; Fuermaier, 2016{#5208}; Suhr, 2011{#10849}; Fuermaier, 2024{#11004}; Robinson, 2025{#11099}; Robinson, 2023{#14273})</t>
+          <t>20 studies (Abramson, 2023{#5}; Becke, 2023{#58}; Berger, 2021{#68}; Courrege, 2019{#164}; Musso, 2016{#646}; Potts, 2022{#733}; Quinn, 2003{#745}; Ramachandran, 2019{#750}; Robinson, 2023{#777}; Smith, 2017{#863}; Sollman, 2010{#872}; Spenceley, 2022{#883}; Young, 2011{#1015}; Harrison, 2020{#4042}; Morey, 2019{#4321}; Fuermaier, 2016{#5208}; Suhr, 2011{#10849}; Fuermaier, 2024{#11004}; Robinson, 2025{#11099}; Robinson, 2023{#14273})</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">

</xml_diff>